<commit_message>
Update Data collection.xlsx with new data
</commit_message>
<xml_diff>
--- a/Evaluation Folder/Output/Data collection.xlsx
+++ b/Evaluation Folder/Output/Data collection.xlsx
@@ -8,27 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a0f9b98384af4391/Desktop/Morph/Python/Single/Tecan/Tecan_Reader/Evaluation Folder/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD3F05326D9DCBA705D3088B35299F652" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B46C5735-66BF-4D84-AEA3-2536870C6AEF}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD3B0D260726160F2443088B35299F08A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8EA0643-DF98-43CF-9B06-F11AAC02871D}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -419,7 +406,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G7"/>
+      <selection activeCell="A2" sqref="A2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update Data collection.xlsx with modified output data
</commit_message>
<xml_diff>
--- a/Evaluation Folder/Output/Data collection.xlsx
+++ b/Evaluation Folder/Output/Data collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a0f9b98384af4391/Desktop/Morph/Python/Single/Tecan/Tecan_Reader/Evaluation Folder/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD3B0D260726160F2443088B35299F08A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8EA0643-DF98-43CF-9B06-F11AAC02871D}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD3F0550342B90E52573088B35299F25A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{616DA75A-D861-4294-8F92-303E54F8C179}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G4"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>